<commit_message>
letter shaped profiles, population ranks
</commit_message>
<xml_diff>
--- a/data/questionnaires/questionnaire_Cao.xlsx
+++ b/data/questionnaires/questionnaire_Cao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="139">
   <si>
     <t xml:space="preserve">factor_name</t>
   </si>
@@ -28,7 +28,10 @@
     <t xml:space="preserve">item</t>
   </si>
   <si>
-    <t xml:space="preserve">capability</t>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity</t>
   </si>
   <si>
     <t xml:space="preserve">preference</t>
@@ -40,220 +43,400 @@
     <t xml:space="preserve">skl_negotiation</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.1.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_persuasion</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.1.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_speech_clarity</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.b.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_speech_recognition</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.b.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">engineering</t>
   </si>
   <si>
     <t xml:space="preserve">knw_industrial_design</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.3.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_building_and_construction</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.3.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_mechanical</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.3.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_production_and_processing</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.2.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">health_science</t>
   </si>
   <si>
     <t xml:space="preserve">knw_medicine_and_dentistry</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.5.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_biology</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.4.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_therapy_and_counseling</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.5.b</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_psychology</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.4.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">spatial_abilities</t>
   </si>
   <si>
     <t xml:space="preserve">abl_peripheral_vision</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.a.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_glare_sensitivity</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.a.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_spatial_orientation</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.1.f.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_transportation</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.10</t>
+  </si>
+  <si>
     <t xml:space="preserve">management</t>
   </si>
   <si>
     <t xml:space="preserve">skl_management_of_material_resources</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.5.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_management_of_personal_resources</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.5.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_management_of_financial_resources</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.5.b</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_personnel_and_human_resources</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.1.f</t>
+  </si>
+  <si>
     <t xml:space="preserve">arts_and_humanities</t>
   </si>
   <si>
     <t xml:space="preserve">knw_history_and_archeology</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.7.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_fine_arts</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.7.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_philosophy_and_theology</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.7.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_geography</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.4.g</t>
+  </si>
+  <si>
     <t xml:space="preserve">mathematics</t>
   </si>
   <si>
     <t xml:space="preserve">skl_pure_mathematics</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.A.1.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_number_facility</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.1.c.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_mathematical_reasoning</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.1.c.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_applied_mathematics</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.4.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">business</t>
   </si>
   <si>
     <t xml:space="preserve">knw_sales_and_marketing</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.1.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_customer_and_personal_service</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.1.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_economics_and_accounting</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.1.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_communications_and_media</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.9.b</t>
+  </si>
+  <si>
     <t xml:space="preserve">perception</t>
   </si>
   <si>
     <t xml:space="preserve">abl_hearing_sensitivity</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.b.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_auditory_attention</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.b.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_visual_color_discrimination</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.4.a.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_operations_monitoring</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.g</t>
+  </si>
+  <si>
     <t xml:space="preserve">robustness</t>
   </si>
   <si>
     <t xml:space="preserve">abl_stamina</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.b.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_gross_body_coordination</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.c.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_gross_body_equilibrium</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.c.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_dynamic_strength</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.a.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_static_strength</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.a.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_extent_flexibility</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.c.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_trunk_strength</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.3.a.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_speed_of_limb_movement</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.2.c.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">mechanical_skills</t>
   </si>
   <si>
     <t xml:space="preserve">skl_repairing</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.l</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_equipment_maintenance</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.j</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_equipment_selection</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.c</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_installation</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.d</t>
+  </si>
+  <si>
     <t xml:space="preserve">administrative_skills</t>
   </si>
   <si>
     <t xml:space="preserve">knw_administrative</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.1.b</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_computers_and_electronics</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.3.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">knw_telecommunications</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.C.9.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_reading_comprehension</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.A.1.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">analytical_skills</t>
   </si>
   <si>
     <t xml:space="preserve">skl_programming</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.e</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_inductive_reasoning</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.1.b.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">skl_operations_analysis</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/2.B.3.a</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_written_comprehension</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.1.a.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">dexterity</t>
   </si>
   <si>
     <t xml:space="preserve">abl_arm_hand_steadiness</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.2.a.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_manual_dexterity</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.2.a.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_control_precision</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.2.b.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">abl_multilimb_coordination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.onetonline.org/find/descriptor/result/1.A.2.b.2</t>
   </si>
 </sst>
 </file>
@@ -540,16 +723,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,851 +749,1032 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="E2" s="2" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>83</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>67</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="2" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="E10" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>67</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E11" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>67</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E12" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>83</v>
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E13" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>83</v>
+        <v>33</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E14" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="E15" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>67</v>
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E16" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="E17" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D18" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E18" s="2" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>67</v>
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E19" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>83</v>
+        <v>46</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="2" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E21" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D22" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E22" s="2" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D23" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E23" s="2" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>83</v>
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E24" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="E25" s="2" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>83</v>
+        <v>60</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D26" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E26" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="2" t="n">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E27" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>83</v>
+        <v>64</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D28" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E28" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>83</v>
+        <v>66</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D29" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E29" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="D30" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E30" s="2" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="2" t="n">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="D31" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E31" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="2" t="n">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D32" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E32" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="2" t="n">
-        <v>67</v>
+        <v>75</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D33" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E33" s="2" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="E34" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="E35" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="2" t="n">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="D36" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E36" s="2" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="2" t="n">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D37" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E37" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>67</v>
+        <v>87</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D38" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E38" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>67</v>
+        <v>89</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D39" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E39" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="E40" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="2" t="n">
-        <v>67</v>
+        <v>93</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D41" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E41" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="2" t="n">
-        <v>67</v>
+        <v>95</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D42" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E42" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="E43" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="2" t="n">
-        <v>67</v>
+        <v>99</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D44" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E44" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="2" t="n">
-        <v>67</v>
+        <v>101</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D46" s="2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="E47" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C48" s="2" t="n">
-        <v>83</v>
+        <v>108</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D48" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E48" s="2" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="E49" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C50" s="2" t="n">
-        <v>83</v>
+        <v>113</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D50" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E50" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="2" t="n">
-        <v>83</v>
+        <v>115</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="D51" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E51" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="2" t="n">
-        <v>83</v>
+        <v>117</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D52" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E52" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="2" t="n">
-        <v>83</v>
+        <v>119</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="D53" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E53" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="2" t="n">
-        <v>67</v>
+        <v>122</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D54" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E54" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="2" t="n">
-        <v>83</v>
+        <v>124</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="D55" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E55" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="2" t="n">
-        <v>67</v>
+        <v>126</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D56" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="E56" s="2" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C57" s="2" t="n">
-        <v>83</v>
+        <v>128</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="D57" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="E57" s="2" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D58" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D58" s="2" t="n">
+      <c r="E58" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C59" s="2" t="n">
-        <v>67</v>
+        <v>133</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="E60" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" s="2" t="n">
-        <v>67</v>
+        <v>137</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>67</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>